<commit_message>
Agregado de scripts, logs y estructura documental al repositorio
</commit_message>
<xml_diff>
--- a/resumen_archivo.xlsx
+++ b/resumen_archivo.xlsx
@@ -417,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,6 +471,17 @@
         </is>
       </c>
     </row>
+    <row r="13"/>
+    <row r="14">
+      <c r="A14" t="inlineStr"/>
+      <c r="B14" t="inlineStr"/>
+      <c r="C14" t="inlineStr"/>
+      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="inlineStr"/>
+      <c r="G14" t="inlineStr"/>
+      <c r="H14" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Versión inicial del sistema de archivado automático
</commit_message>
<xml_diff>
--- a/resumen_archivo.xlsx
+++ b/resumen_archivo.xlsx
@@ -417,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H106"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,16 +471,16 @@
         </is>
       </c>
     </row>
-    <row r="13"/>
-    <row r="14">
-      <c r="A14" t="inlineStr"/>
-      <c r="B14" t="inlineStr"/>
-      <c r="C14" t="inlineStr"/>
-      <c r="D14" t="inlineStr"/>
-      <c r="E14" t="inlineStr"/>
-      <c r="F14" t="inlineStr"/>
-      <c r="G14" t="inlineStr"/>
-      <c r="H14" t="inlineStr"/>
+    <row r="105"/>
+    <row r="106">
+      <c r="A106" t="inlineStr"/>
+      <c r="B106" t="inlineStr"/>
+      <c r="C106" t="inlineStr"/>
+      <c r="D106" t="inlineStr"/>
+      <c r="E106" t="inlineStr"/>
+      <c r="F106" t="inlineStr"/>
+      <c r="G106" t="inlineStr"/>
+      <c r="H106" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
feat: agrego archivado_auditable.py con lógica de auditoría y colisión de hash
</commit_message>
<xml_diff>
--- a/resumen_archivo.xlsx
+++ b/resumen_archivo.xlsx
@@ -417,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H106"/>
+  <dimension ref="A1:H158"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,16 +471,379 @@
         </is>
       </c>
     </row>
-    <row r="105"/>
-    <row r="106">
-      <c r="A106" t="inlineStr"/>
-      <c r="B106" t="inlineStr"/>
-      <c r="C106" t="inlineStr"/>
-      <c r="D106" t="inlineStr"/>
-      <c r="E106" t="inlineStr"/>
-      <c r="F106" t="inlineStr"/>
-      <c r="G106" t="inlineStr"/>
-      <c r="H106" t="inlineStr"/>
+    <row r="120">
+      <c r="H120" t="inlineStr">
+        <is>
+          <t>b14db56411e67896f5ff2c4f229286345bf094f7ba8e071ff8e147b45ae8429c</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="H121" t="inlineStr">
+        <is>
+          <t>6fda0e78c3d830a954e30387e5b82a080d53946d8b72cb15b6bd0ff4cafc8e3f</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="H122" t="inlineStr">
+        <is>
+          <t>ed16dc78ccc4d5510d49c402182be0daaaa19b8f4d47f1b5b7d42e40515b38f3</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="H123" t="inlineStr">
+        <is>
+          <t>4279991429b94b829db5146e62919e924afc9d91b69667262477b1ec36b31a77</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="H124" t="inlineStr">
+        <is>
+          <t>328ff33e59c9dfab850d87d78e9891f5623af781e97f83493e43a38cd0a7eefc</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="H125" t="inlineStr">
+        <is>
+          <t>481056ec408fcc256f1a4769dda26e32fe9f3339a9731459d8b3b0bffb70b01c</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="H126" t="inlineStr">
+        <is>
+          <t>b7dfbe557999e5bd6347fa698290f28ddaa0bfb3841f1d9023ce82a81d672898</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="H127" t="inlineStr">
+        <is>
+          <t>b14db56411e67896f5ff2c4f229286345bf094f7ba8e071ff8e147b45ae8429c</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="H128" t="inlineStr">
+        <is>
+          <t>b14db56411e67896f5ff2c4f229286345bf094f7ba8e071ff8e147b45ae8429c</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="H129" t="inlineStr">
+        <is>
+          <t>b14db56411e67896f5ff2c4f229286345bf094f7ba8e071ff8e147b45ae8429c</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="H130" t="inlineStr">
+        <is>
+          <t>b14db56411e67896f5ff2c4f229286345bf094f7ba8e071ff8e147b45ae8429c</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="H131" t="inlineStr">
+        <is>
+          <t>b14db56411e67896f5ff2c4f229286345bf094f7ba8e071ff8e147b45ae8429c</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="H132" t="inlineStr">
+        <is>
+          <t>b14db56411e67896f5ff2c4f229286345bf094f7ba8e071ff8e147b45ae8429c</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="H133" t="inlineStr">
+        <is>
+          <t>608d9d68c0118168924b8293ff6c809174e4eb758f7ee444c7b5b270c9cccc09</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="H134" t="inlineStr">
+        <is>
+          <t>f76c3a80b9920e968242872d921309f1665bf5d5dff9091ab197281379c748cc</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="H135" t="inlineStr">
+        <is>
+          <t>b14db56411e67896f5ff2c4f229286345bf094f7ba8e071ff8e147b45ae8429c</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="H136" t="inlineStr">
+        <is>
+          <t>08ef215b699ba7e5b5996a170c1e065b066acdd0d3501e700977bd527abdf216</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="H137" t="inlineStr">
+        <is>
+          <t>6fda0e78c3d830a954e30387e5b82a080d53946d8b72cb15b6bd0ff4cafc8e3f</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="H138" t="inlineStr">
+        <is>
+          <t>ed16dc78ccc4d5510d49c402182be0daaaa19b8f4d47f1b5b7d42e40515b38f3</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="H139" t="inlineStr">
+        <is>
+          <t>4279991429b94b829db5146e62919e924afc9d91b69667262477b1ec36b31a77</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="H140" t="inlineStr">
+        <is>
+          <t>328ff33e59c9dfab850d87d78e9891f5623af781e97f83493e43a38cd0a7eefc</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="H141" t="inlineStr">
+        <is>
+          <t>481056ec408fcc256f1a4769dda26e32fe9f3339a9731459d8b3b0bffb70b01c</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="H142" t="inlineStr">
+        <is>
+          <t>b7dfbe557999e5bd6347fa698290f28ddaa0bfb3841f1d9023ce82a81d672898</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="H143" t="inlineStr">
+        <is>
+          <t>f94b5f7c7abeecf24d8b2913fbdaf75ce15889afafb0b2b34a741232deceff34</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr"/>
+      <c r="B144" t="inlineStr"/>
+      <c r="C144" t="inlineStr"/>
+      <c r="D144" t="inlineStr"/>
+      <c r="E144" t="inlineStr"/>
+      <c r="F144" t="inlineStr"/>
+      <c r="G144" t="inlineStr"/>
+      <c r="H144" t="inlineStr">
+        <is>
+          <t>608d9d68c0118168924b8293ff6c809174e4eb758f7ee444c7b5b270c9cccc09</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr"/>
+      <c r="B145" t="inlineStr"/>
+      <c r="C145" t="inlineStr"/>
+      <c r="D145" t="inlineStr"/>
+      <c r="E145" t="inlineStr"/>
+      <c r="F145" t="inlineStr"/>
+      <c r="G145" t="inlineStr"/>
+      <c r="H145" t="inlineStr">
+        <is>
+          <t>1a9a150697d1f0d7f3165dc3baee84dd4e5401cbef7aabb5e6f24a634fd33d8c</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr"/>
+      <c r="B146" t="inlineStr"/>
+      <c r="C146" t="inlineStr"/>
+      <c r="D146" t="inlineStr"/>
+      <c r="E146" t="inlineStr"/>
+      <c r="F146" t="inlineStr"/>
+      <c r="G146" t="inlineStr"/>
+      <c r="H146" t="inlineStr">
+        <is>
+          <t>6fda0e78c3d830a954e30387e5b82a080d53946d8b72cb15b6bd0ff4cafc8e3f</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr"/>
+      <c r="B147" t="inlineStr"/>
+      <c r="C147" t="inlineStr"/>
+      <c r="D147" t="inlineStr"/>
+      <c r="E147" t="inlineStr"/>
+      <c r="F147" t="inlineStr"/>
+      <c r="G147" t="inlineStr"/>
+      <c r="H147" t="inlineStr">
+        <is>
+          <t>08ef215b699ba7e5b5996a170c1e065b066acdd0d3501e700977bd527abdf216</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr"/>
+      <c r="B148" t="inlineStr"/>
+      <c r="C148" t="inlineStr"/>
+      <c r="D148" t="inlineStr"/>
+      <c r="E148" t="inlineStr"/>
+      <c r="F148" t="inlineStr"/>
+      <c r="G148" t="inlineStr"/>
+      <c r="H148" t="inlineStr">
+        <is>
+          <t>87563d53f229c2b65c15c663a437052d52b997e5cec04dd43b53ab4f6fbd1095</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr"/>
+      <c r="B149" t="inlineStr"/>
+      <c r="C149" t="inlineStr"/>
+      <c r="D149" t="inlineStr"/>
+      <c r="E149" t="inlineStr"/>
+      <c r="F149" t="inlineStr"/>
+      <c r="G149" t="inlineStr"/>
+      <c r="H149" t="inlineStr"/>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr"/>
+      <c r="B150" t="inlineStr"/>
+      <c r="C150" t="inlineStr"/>
+      <c r="D150" t="inlineStr"/>
+      <c r="E150" t="inlineStr"/>
+      <c r="F150" t="inlineStr"/>
+      <c r="G150" t="inlineStr"/>
+      <c r="H150" t="inlineStr">
+        <is>
+          <t>eb5e37fbe5f44b34580e145ebb8ea7878183037ab930744dfbdf161b966c748d</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr"/>
+      <c r="B151" t="inlineStr"/>
+      <c r="C151" t="inlineStr"/>
+      <c r="D151" t="inlineStr"/>
+      <c r="E151" t="inlineStr"/>
+      <c r="F151" t="inlineStr"/>
+      <c r="G151" t="inlineStr"/>
+      <c r="H151" t="inlineStr">
+        <is>
+          <t>ed16dc78ccc4d5510d49c402182be0daaaa19b8f4d47f1b5b7d42e40515b38f3</t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr"/>
+      <c r="B152" t="inlineStr"/>
+      <c r="C152" t="inlineStr"/>
+      <c r="D152" t="inlineStr"/>
+      <c r="E152" t="inlineStr"/>
+      <c r="F152" t="inlineStr"/>
+      <c r="G152" t="inlineStr"/>
+      <c r="H152" t="inlineStr">
+        <is>
+          <t>2ecc37d6eab868aa60d18a2cd86c54ef7f79f6be1fb99f22fcdfd22c5ad46cb9</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr"/>
+      <c r="B153" t="inlineStr"/>
+      <c r="C153" t="inlineStr"/>
+      <c r="D153" t="inlineStr"/>
+      <c r="E153" t="inlineStr"/>
+      <c r="F153" t="inlineStr"/>
+      <c r="G153" t="inlineStr"/>
+      <c r="H153" t="inlineStr">
+        <is>
+          <t>24c589d8df102d0fbbcae4cb4339c90d98e62073c0902b19327836ea9f5c4e9a</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr"/>
+      <c r="B154" t="inlineStr"/>
+      <c r="C154" t="inlineStr"/>
+      <c r="D154" t="inlineStr"/>
+      <c r="E154" t="inlineStr"/>
+      <c r="F154" t="inlineStr"/>
+      <c r="G154" t="inlineStr"/>
+      <c r="H154" t="inlineStr">
+        <is>
+          <t>4279991429b94b829db5146e62919e924afc9d91b69667262477b1ec36b31a77</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr"/>
+      <c r="B155" t="inlineStr"/>
+      <c r="C155" t="inlineStr"/>
+      <c r="D155" t="inlineStr"/>
+      <c r="E155" t="inlineStr"/>
+      <c r="F155" t="inlineStr"/>
+      <c r="G155" t="inlineStr"/>
+      <c r="H155" t="inlineStr">
+        <is>
+          <t>328ff33e59c9dfab850d87d78e9891f5623af781e97f83493e43a38cd0a7eefc</t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr"/>
+      <c r="B156" t="inlineStr"/>
+      <c r="C156" t="inlineStr"/>
+      <c r="D156" t="inlineStr"/>
+      <c r="E156" t="inlineStr"/>
+      <c r="F156" t="inlineStr"/>
+      <c r="G156" t="inlineStr"/>
+      <c r="H156" t="inlineStr">
+        <is>
+          <t>481056ec408fcc256f1a4769dda26e32fe9f3339a9731459d8b3b0bffb70b01c</t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr"/>
+      <c r="B157" t="inlineStr"/>
+      <c r="C157" t="inlineStr"/>
+      <c r="D157" t="inlineStr"/>
+      <c r="E157" t="inlineStr"/>
+      <c r="F157" t="inlineStr"/>
+      <c r="G157" t="inlineStr"/>
+      <c r="H157" t="inlineStr">
+        <is>
+          <t>b7dfbe557999e5bd6347fa698290f28ddaa0bfb3841f1d9023ce82a81d672898</t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr"/>
+      <c r="B158" t="inlineStr"/>
+      <c r="C158" t="inlineStr"/>
+      <c r="D158" t="inlineStr"/>
+      <c r="E158" t="inlineStr"/>
+      <c r="F158" t="inlineStr"/>
+      <c r="G158" t="inlineStr"/>
+      <c r="H158" t="inlineStr">
+        <is>
+          <t>f94b5f7c7abeecf24d8b2913fbdaf75ce15889afafb0b2b34a741232deceff34</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>